<commit_message>
refcode2 in excel util
</commit_message>
<xml_diff>
--- a/D:\test excel\2_IDP May Refcodes for upload.xlsx
+++ b/D:\test excel\2_IDP May Refcodes for upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoe/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75460090-4E6C-DB4E-B204-FE7B5DA03651}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA1A9CA-F678-B449-AD0C-D7BDE4403AE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3780" yWindow="500" windowWidth="24640" windowHeight="13560" xr2:uid="{018ACE7B-E409-8A49-BD21-E7C1F3D5D035}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Receipt ID</t>
   </si>
@@ -90,25 +90,67 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Fishers</t>
-  </si>
-  <si>
-    <t>Guba</t>
-  </si>
-  <si>
-    <t>helloguba@gmail.com</t>
-  </si>
-  <si>
-    <t>435  Ave #806</t>
-  </si>
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>AB99999810702417777</t>
-  </si>
-  <si>
-    <t>testRefcode5</t>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Kidd</t>
+  </si>
+  <si>
+    <t>McKenzie</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>backontrack.fr.042821</t>
+  </si>
+  <si>
+    <t>Martha</t>
+  </si>
+  <si>
+    <t>Lemert</t>
+  </si>
+  <si>
+    <t>Fort Wayne</t>
+  </si>
+  <si>
+    <t>lemertmartha@gmail.com</t>
+  </si>
+  <si>
+    <t>Reference Code 2</t>
+  </si>
+  <si>
+    <t>TEST 2</t>
+  </si>
+  <si>
+    <t>TEST 1</t>
+  </si>
+  <si>
+    <t>GB195892342</t>
+  </si>
+  <si>
+    <t>TEST Rd</t>
+  </si>
+  <si>
+    <t>newdonor@bethelu.edu</t>
+  </si>
+  <si>
+    <t>TESTbackontrack.fr.042821</t>
+  </si>
+  <si>
+    <t>newdonor@gmail.com</t>
+  </si>
+  <si>
+    <t>RedistrictingEOM.FR.05.27.21.</t>
+  </si>
+  <si>
+    <t>TEST 3</t>
+  </si>
+  <si>
+    <t>KK195892342</t>
+  </si>
+  <si>
+    <t>AB10958920755555</t>
   </si>
 </sst>
 </file>
@@ -478,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8CB9B3-7067-2249-AC6E-C70455D95340}">
-  <dimension ref="A1:O114"/>
+  <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,7 +535,7 @@
     <col min="15" max="15" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -522,16 +564,16 @@
         <v>9</v>
       </c>
       <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
       </c>
       <c r="N1" t="s">
         <v>13</v>
@@ -539,94 +581,229 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1">
-        <v>44566.181064814817</v>
+        <v>44344.184224537035</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>20.21</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
       </c>
       <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2">
+        <v>38201</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44344.184224537035</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <v>46845</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44344.184224537035</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4">
+        <v>46845</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44344.184224537035</v>
+      </c>
+      <c r="C5">
+        <v>20.21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2">
-        <v>46203</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5">
+        <v>38201</v>
+      </c>
+      <c r="M5" t="s">
         <v>17</v>
       </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2">
-        <v>3176084314</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
@@ -924,12 +1101,14 @@
       <c r="B114" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O114">
-    <sortCondition ref="B2:B114"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O114">
+    <sortCondition ref="B3:B114"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{B58C160E-0B5C-F140-9708-C3658D373191}"/>
+    <hyperlink ref="N4" r:id="rId1" xr:uid="{B3CD58DF-85D1-7D4B-A45D-BDEE7BAA45C4}"/>
+    <hyperlink ref="N5" r:id="rId2" xr:uid="{A68259DA-39BC-3942-8B8F-718C101428AD}"/>
+    <hyperlink ref="N2" r:id="rId3" xr:uid="{D35709CE-6D4F-A342-BC05-86662319991D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refcode 2 updating when reupload stuff
</commit_message>
<xml_diff>
--- a/D:\test excel\2_IDP May Refcodes for upload.xlsx
+++ b/D:\test excel\2_IDP May Refcodes for upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoe/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA1A9CA-F678-B449-AD0C-D7BDE4403AE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651CE85A-D125-0949-BBF6-79B8A3BD8EA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3780" yWindow="500" windowWidth="24640" windowHeight="13560" xr2:uid="{018ACE7B-E409-8A49-BD21-E7C1F3D5D035}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Receipt ID</t>
   </si>
@@ -90,74 +90,80 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>Kidd</t>
-  </si>
-  <si>
-    <t>McKenzie</t>
-  </si>
-  <si>
-    <t>TN</t>
-  </si>
-  <si>
-    <t>backontrack.fr.042821</t>
-  </si>
-  <si>
-    <t>Martha</t>
-  </si>
-  <si>
-    <t>Lemert</t>
-  </si>
-  <si>
-    <t>Fort Wayne</t>
-  </si>
-  <si>
-    <t>lemertmartha@gmail.com</t>
-  </si>
-  <si>
     <t>Reference Code 2</t>
   </si>
   <si>
-    <t>TEST 2</t>
-  </si>
-  <si>
-    <t>TEST 1</t>
-  </si>
-  <si>
-    <t>GB195892342</t>
-  </si>
-  <si>
-    <t>TEST Rd</t>
-  </si>
-  <si>
-    <t>newdonor@bethelu.edu</t>
-  </si>
-  <si>
-    <t>TESTbackontrack.fr.042821</t>
-  </si>
-  <si>
-    <t>newdonor@gmail.com</t>
-  </si>
-  <si>
-    <t>RedistrictingEOM.FR.05.27.21.</t>
-  </si>
-  <si>
-    <t>TEST 3</t>
-  </si>
-  <si>
-    <t>KK195892342</t>
-  </si>
-  <si>
-    <t>AB10958920755555</t>
+    <t>AB191624287</t>
+  </si>
+  <si>
+    <t>Reba</t>
+  </si>
+  <si>
+    <t>Wooden</t>
+  </si>
+  <si>
+    <t>113 Severn Drive</t>
+  </si>
+  <si>
+    <t>Greenwood</t>
+  </si>
+  <si>
+    <t>rboydw@gmsil.com</t>
+  </si>
+  <si>
+    <t>2.22.21.EOM1.</t>
+  </si>
+  <si>
+    <t>AB191627990</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>Braun</t>
+  </si>
+  <si>
+    <t>11 Parker Road</t>
+  </si>
+  <si>
+    <t>Arlington</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>lbraun@verizon.net</t>
+  </si>
+  <si>
+    <t>AB191641364</t>
+  </si>
+  <si>
+    <t>Kathleen</t>
+  </si>
+  <si>
+    <t>Clausen</t>
+  </si>
+  <si>
+    <t>7005 Dean Rd.</t>
+  </si>
+  <si>
+    <t>Indianapolis</t>
+  </si>
+  <si>
+    <t>kathleen.j.clausen@gmail.com</t>
+  </si>
+  <si>
+    <t>TEST 9</t>
+  </si>
+  <si>
+    <t>TEST 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -167,14 +173,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,17 +195,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8CB9B3-7067-2249-AC6E-C70455D95340}">
-  <dimension ref="A1:P114"/>
+  <dimension ref="A1:P113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,8 +526,8 @@
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.1640625" customWidth="1"/>
-    <col min="15" max="15" width="38" customWidth="1"/>
+    <col min="11" max="11" width="40.1640625" customWidth="1"/>
+    <col min="16" max="16" width="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -555,16 +550,16 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -587,57 +582,60 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1">
-        <v>44344.184224537035</v>
+        <v>44338.17931712963</v>
       </c>
       <c r="C2">
-        <v>20.21</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L2">
-        <v>38201</v>
+        <v>46142</v>
       </c>
       <c r="M2" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>32</v>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2">
+        <v>3177975892</v>
       </c>
       <c r="P2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>44344.184224537035</v>
+        <v>44338.179351851853</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -646,132 +644,88 @@
         <v>15</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
       <c r="L3">
-        <v>46845</v>
+        <v>2474</v>
       </c>
       <c r="M3" t="s">
         <v>17</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="O3">
+        <v>7816462999</v>
       </c>
       <c r="P3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1">
-        <v>44344.184224537035</v>
+        <v>44338.179456018515</v>
       </c>
       <c r="C4">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
         <v>16</v>
       </c>
       <c r="L4">
-        <v>46845</v>
+        <v>46220</v>
       </c>
       <c r="M4" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>34</v>
+      <c r="N4" t="s">
+        <v>38</v>
       </c>
       <c r="P4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44344.184224537035</v>
-      </c>
-      <c r="C5">
-        <v>20.21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5">
-        <v>38201</v>
-      </c>
-      <c r="M5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P5" t="s">
-        <v>33</v>
-      </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
@@ -1097,19 +1051,11 @@
     <row r="113" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B113" s="1"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B114" s="1"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O114">
-    <sortCondition ref="B3:B114"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:P113">
+    <sortCondition ref="B3:B113"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="N4" r:id="rId1" xr:uid="{B3CD58DF-85D1-7D4B-A45D-BDEE7BAA45C4}"/>
-    <hyperlink ref="N5" r:id="rId2" xr:uid="{A68259DA-39BC-3942-8B8F-718C101428AD}"/>
-    <hyperlink ref="N2" r:id="rId3" xr:uid="{D35709CE-6D4F-A342-BC05-86662319991D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>